<commit_message>
breast to breast (early)
</commit_message>
<xml_diff>
--- a/docs/metaData_v4.xlsx
+++ b/docs/metaData_v4.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Data Sub-Category-3</t>
   </si>
   <si>
-    <t xml:space="preserve">Breast Cancer</t>
+    <t xml:space="preserve">Breast (early) Cancer</t>
   </si>
   <si>
     <t xml:space="preserve">Ovarian Cancer</t>
@@ -1918,10 +1918,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="V9" activeCellId="0" sqref="V9"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>